<commit_message>
add model for hall transitions time
</commit_message>
<xml_diff>
--- a/app/data/HallsTime-good.xlsx
+++ b/app/data/HallsTime-good.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgijmamarin/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgijmamarin/Desktop/Figaro_bot/Figaro_bot-2/Figaro/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67ED2AE-050B-3A47-A78A-579F9D728477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B96A902-9DF0-B34B-87AD-A78030DD85DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="16440" windowHeight="18580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>Камерный зал филармонии</t>
   </si>
@@ -44,6 +57,9 @@
   </si>
   <si>
     <t>Сад Вайнера — 2021 год</t>
+  </si>
+  <si>
+    <t>Инфоцентр</t>
   </si>
 </sst>
 </file>
@@ -62,6 +78,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -72,7 +89,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -95,11 +112,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -109,6 +137,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -412,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="J2" sqref="J2:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -424,7 +455,7 @@
     <col min="2" max="9" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -449,8 +480,11 @@
       <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,8 +512,11 @@
       <c r="I2" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -507,8 +544,11 @@
       <c r="I3" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -536,8 +576,11 @@
       <c r="I4" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -565,8 +608,11 @@
       <c r="I5" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -594,8 +640,11 @@
       <c r="I6" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -623,8 +672,11 @@
       <c r="I7" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -652,8 +704,11 @@
       <c r="I8" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -679,6 +734,41 @@
         <v>9</v>
       </c>
       <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix dormat at recomendation offprog at route list
</commit_message>
<xml_diff>
--- a/app/data/HallsTime-good.xlsx
+++ b/app/data/HallsTime-good.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgijmamarin/Desktop/Figaro_bot/Figaro_bot-2/Figaro/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B96A902-9DF0-B34B-87AD-A78030DD85DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AB1AE3-90D1-4C42-AF3D-0AAC2975048C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="16440" windowHeight="18580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -138,7 +138,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -512,8 +512,8 @@
       <c r="I2" s="3">
         <v>2</v>
       </c>
-      <c r="J2">
-        <v>0</v>
+      <c r="J2" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -544,8 +544,8 @@
       <c r="I3" s="3">
         <v>14</v>
       </c>
-      <c r="J3">
-        <v>0</v>
+      <c r="J3" s="3">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -576,8 +576,8 @@
       <c r="I4" s="3">
         <v>2</v>
       </c>
-      <c r="J4">
-        <v>0</v>
+      <c r="J4" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -608,8 +608,8 @@
       <c r="I5" s="3">
         <v>9</v>
       </c>
-      <c r="J5">
-        <v>0</v>
+      <c r="J5" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -640,8 +640,8 @@
       <c r="I6" s="3">
         <v>7</v>
       </c>
-      <c r="J6">
-        <v>0</v>
+      <c r="J6" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -672,8 +672,8 @@
       <c r="I7" s="3">
         <v>2</v>
       </c>
-      <c r="J7">
-        <v>0</v>
+      <c r="J7" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -704,8 +704,8 @@
       <c r="I8" s="3">
         <v>9</v>
       </c>
-      <c r="J8">
-        <v>0</v>
+      <c r="J8" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -736,7 +736,7 @@
       <c r="I9" s="3">
         <v>0</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="3">
         <v>0</v>
       </c>
     </row>
@@ -744,28 +744,28 @@
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3">
+        <v>14</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3">
+        <v>9</v>
+      </c>
+      <c r="F10" s="3">
+        <v>7</v>
+      </c>
+      <c r="G10" s="3">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3">
+        <v>9</v>
+      </c>
+      <c r="I10" s="3">
         <v>0</v>
       </c>
       <c r="J10">

</xml_diff>